<commit_message>
did some slight adjustments
</commit_message>
<xml_diff>
--- a/UploadArtifacts/DaniëlGroeneweg_532508_unity_fundamentals_personal_project_template.xlsx
+++ b/UploadArtifacts/DaniëlGroeneweg_532508_unity_fundamentals_personal_project_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danie\Desktop\Coding\Git\Walking_Simulator_CMGT\UploadArtifacts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5888A4C-9C0F-4CFD-9E88-224490BE07B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7F07399-4A35-4E84-8C5F-8565211DB5FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Step 1 - Requirements check" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="71">
   <si>
     <t>Preconditions</t>
   </si>
@@ -283,6 +283,9 @@
   </si>
   <si>
     <t>Properly use anchors, positions, and layouts for the HUD and in-game menus, such as they are resolution-independent.</t>
+  </si>
+  <si>
+    <t>[</t>
   </si>
 </sst>
 </file>
@@ -445,7 +448,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <extLst>
@@ -504,6 +507,10 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" indent="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -552,7 +559,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -886,8 +892,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+    <sheetView topLeftCell="A2" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -988,22 +994,27 @@
         <v>1</v>
       </c>
     </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>70</v>
+      </c>
+    </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+      <c r="A15" s="22" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" s="9" t="s">
+      <c r="A16" s="23" t="s">
         <v>30</v>
       </c>
       <c r="B16" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -1011,7 +1022,7 @@
         <v>31</v>
       </c>
       <c r="B17" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -1023,7 +1034,7 @@
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="38" t="s">
+      <c r="A19" s="22" t="s">
         <v>33</v>
       </c>
     </row>
@@ -1058,7 +1069,7 @@
         <v>32</v>
       </c>
       <c r="B23" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
@@ -1066,7 +1077,7 @@
         <v>5</v>
       </c>
       <c r="B24" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E24" s="11"/>
     </row>
@@ -1095,8 +1106,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F77FDBE-4564-4278-9755-9E7B4B955105}">
   <dimension ref="A1:G25"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1110,17 +1121,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="25"/>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
-      <c r="E1" s="25"/>
-      <c r="F1" s="25"/>
+      <c r="B1" s="27"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
+      <c r="F1" s="27"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="22" t="s">
+      <c r="A3" s="24" t="s">
         <v>6</v>
       </c>
       <c r="B3" s="4" t="s">
@@ -1135,13 +1146,13 @@
       <c r="E3" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="F3" s="23" t="s">
+      <c r="F3" s="25" t="s">
         <v>40</v>
       </c>
       <c r="G3" s="3"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="22"/>
+      <c r="A4" s="24"/>
       <c r="B4" s="5" t="s">
         <v>8</v>
       </c>
@@ -1154,70 +1165,70 @@
       <c r="E4" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F4" s="24"/>
+      <c r="F4" s="26"/>
       <c r="G4" s="3"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="G5" s="3"/>
     </row>
     <row r="6" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="26" t="s">
+      <c r="A6" s="28" t="s">
         <v>36</v>
       </c>
-      <c r="B6" s="29" t="s">
+      <c r="B6" s="31" t="s">
         <v>15</v>
       </c>
       <c r="C6" s="15" t="s">
         <v>42</v>
       </c>
-      <c r="D6" s="32" t="s">
+      <c r="D6" s="34" t="s">
         <v>16</v>
       </c>
       <c r="E6" s="15" t="s">
         <v>46</v>
       </c>
-      <c r="F6" s="35" t="s">
+      <c r="F6" s="37" t="s">
         <v>41</v>
       </c>
       <c r="G6" s="3"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="27"/>
-      <c r="B7" s="30"/>
+      <c r="A7" s="29"/>
+      <c r="B7" s="32"/>
       <c r="C7" s="16" t="s">
         <v>43</v>
       </c>
-      <c r="D7" s="33"/>
+      <c r="D7" s="35"/>
       <c r="E7" s="18" t="s">
         <v>47</v>
       </c>
-      <c r="F7" s="36"/>
+      <c r="F7" s="38"/>
       <c r="G7" s="2"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="27"/>
-      <c r="B8" s="30"/>
+      <c r="A8" s="29"/>
+      <c r="B8" s="32"/>
       <c r="C8" s="16" t="s">
         <v>44</v>
       </c>
-      <c r="D8" s="33"/>
+      <c r="D8" s="35"/>
       <c r="E8" s="16" t="s">
         <v>48</v>
       </c>
-      <c r="F8" s="36"/>
+      <c r="F8" s="38"/>
       <c r="G8" s="2"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="28"/>
-      <c r="B9" s="31"/>
+      <c r="A9" s="30"/>
+      <c r="B9" s="33"/>
       <c r="C9" s="17" t="s">
         <v>45</v>
       </c>
-      <c r="D9" s="34"/>
+      <c r="D9" s="36"/>
       <c r="E9" s="17" t="s">
         <v>49</v>
       </c>
-      <c r="F9" s="37"/>
+      <c r="F9" s="39"/>
       <c r="G9" s="2"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -1230,156 +1241,156 @@
       <c r="G10" s="2"/>
     </row>
     <row r="11" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="26" t="s">
+      <c r="A11" s="28" t="s">
         <v>37</v>
       </c>
-      <c r="B11" s="29" t="s">
+      <c r="B11" s="31" t="s">
         <v>15</v>
       </c>
       <c r="C11" s="15" t="s">
         <v>50</v>
       </c>
-      <c r="D11" s="29" t="s">
+      <c r="D11" s="31" t="s">
         <v>16</v>
       </c>
       <c r="E11" s="15" t="s">
         <v>53</v>
       </c>
-      <c r="F11" s="35" t="s">
+      <c r="F11" s="37" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="27"/>
-      <c r="B12" s="30"/>
+      <c r="A12" s="29"/>
+      <c r="B12" s="32"/>
       <c r="C12" s="19" t="s">
         <v>51</v>
       </c>
-      <c r="D12" s="30"/>
+      <c r="D12" s="32"/>
       <c r="E12" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="F12" s="36"/>
+      <c r="F12" s="38"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="28"/>
-      <c r="B13" s="31"/>
+      <c r="A13" s="30"/>
+      <c r="B13" s="33"/>
       <c r="C13" s="20" t="s">
         <v>52</v>
       </c>
-      <c r="D13" s="31"/>
+      <c r="D13" s="33"/>
       <c r="E13" s="14" t="s">
         <v>55</v>
       </c>
-      <c r="F13" s="37"/>
+      <c r="F13" s="39"/>
     </row>
     <row r="15" spans="1:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="26" t="s">
+      <c r="A15" s="28" t="s">
         <v>38</v>
       </c>
-      <c r="B15" s="29" t="s">
+      <c r="B15" s="31" t="s">
         <v>15</v>
       </c>
       <c r="C15" s="15" t="s">
         <v>56</v>
       </c>
-      <c r="D15" s="29" t="s">
+      <c r="D15" s="31" t="s">
         <v>16</v>
       </c>
       <c r="E15" s="15" t="s">
         <v>60</v>
       </c>
-      <c r="F15" s="35" t="s">
+      <c r="F15" s="37" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="27"/>
-      <c r="B16" s="30"/>
+      <c r="A16" s="29"/>
+      <c r="B16" s="32"/>
       <c r="C16" s="19" t="s">
         <v>57</v>
       </c>
-      <c r="D16" s="30"/>
+      <c r="D16" s="32"/>
       <c r="E16" s="13" t="s">
         <v>61</v>
       </c>
-      <c r="F16" s="36"/>
+      <c r="F16" s="38"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="27"/>
-      <c r="B17" s="30"/>
+      <c r="A17" s="29"/>
+      <c r="B17" s="32"/>
       <c r="C17" s="19" t="s">
         <v>58</v>
       </c>
-      <c r="D17" s="30"/>
+      <c r="D17" s="32"/>
       <c r="E17" s="13" t="s">
         <v>62</v>
       </c>
-      <c r="F17" s="36"/>
+      <c r="F17" s="38"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="28"/>
-      <c r="B18" s="31"/>
+      <c r="A18" s="30"/>
+      <c r="B18" s="33"/>
       <c r="C18" s="20" t="s">
         <v>59</v>
       </c>
-      <c r="D18" s="31"/>
+      <c r="D18" s="33"/>
       <c r="E18" s="14"/>
-      <c r="F18" s="37"/>
+      <c r="F18" s="39"/>
     </row>
     <row r="20" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="26" t="s">
+      <c r="A20" s="28" t="s">
         <v>39</v>
       </c>
-      <c r="B20" s="29" t="s">
+      <c r="B20" s="31" t="s">
         <v>15</v>
       </c>
       <c r="C20" s="15" t="s">
         <v>63</v>
       </c>
-      <c r="D20" s="32" t="s">
+      <c r="D20" s="34" t="s">
         <v>16</v>
       </c>
       <c r="E20" s="15" t="s">
         <v>66</v>
       </c>
-      <c r="F20" s="35" t="s">
+      <c r="F20" s="37" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="27"/>
-      <c r="B21" s="30"/>
+      <c r="A21" s="29"/>
+      <c r="B21" s="32"/>
       <c r="C21" s="19" t="s">
         <v>64</v>
       </c>
-      <c r="D21" s="33"/>
+      <c r="D21" s="35"/>
       <c r="E21" s="21" t="s">
         <v>67</v>
       </c>
-      <c r="F21" s="36"/>
+      <c r="F21" s="38"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="27"/>
-      <c r="B22" s="30"/>
+      <c r="A22" s="29"/>
+      <c r="B22" s="32"/>
       <c r="C22" s="19" t="s">
         <v>65</v>
       </c>
-      <c r="D22" s="33"/>
+      <c r="D22" s="35"/>
       <c r="E22" s="13" t="s">
         <v>68</v>
       </c>
-      <c r="F22" s="36"/>
+      <c r="F22" s="38"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="28"/>
-      <c r="B23" s="31"/>
+      <c r="A23" s="30"/>
+      <c r="B23" s="33"/>
       <c r="C23" s="14"/>
-      <c r="D23" s="34"/>
+      <c r="D23" s="36"/>
       <c r="E23" s="20" t="s">
         <v>69</v>
       </c>
-      <c r="F23" s="37"/>
+      <c r="F23" s="39"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="6" t="s">

</xml_diff>

<commit_message>
removed unused files, changed some names
</commit_message>
<xml_diff>
--- a/UploadArtifacts/DaniëlGroeneweg_532508_unity_fundamentals_personal_project_template.xlsx
+++ b/UploadArtifacts/DaniëlGroeneweg_532508_unity_fundamentals_personal_project_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danie\Desktop\Coding\Git\Walking_Simulator_CMGT\UploadArtifacts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7F07399-4A35-4E84-8C5F-8565211DB5FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C0C99C5-FDB0-48D8-8CE4-687C31AA9466}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Step 1 - Requirements check" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="70">
   <si>
     <t>Preconditions</t>
   </si>
@@ -283,9 +283,6 @@
   </si>
   <si>
     <t>Properly use anchors, positions, and layouts for the HUD and in-game menus, such as they are resolution-independent.</t>
-  </si>
-  <si>
-    <t>[</t>
   </si>
 </sst>
 </file>
@@ -334,7 +331,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -374,12 +371,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -507,10 +498,10 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -892,8 +883,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E24"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -994,27 +985,22 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
-        <v>70</v>
-      </c>
-    </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" s="22" t="s">
+      <c r="A15" s="23" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" s="23" t="s">
+      <c r="A16" s="22" t="s">
         <v>30</v>
       </c>
       <c r="B16" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -1022,7 +1008,7 @@
         <v>31</v>
       </c>
       <c r="B17" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -1030,11 +1016,11 @@
         <v>3</v>
       </c>
       <c r="B18" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="22" t="s">
+      <c r="A19" s="23" t="s">
         <v>33</v>
       </c>
     </row>
@@ -1043,7 +1029,7 @@
         <v>34</v>
       </c>
       <c r="B20" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E20" s="11"/>
     </row>
@@ -1052,7 +1038,7 @@
         <v>35</v>
       </c>
       <c r="B21" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E21" s="11"/>
     </row>
@@ -1061,7 +1047,7 @@
         <v>4</v>
       </c>
       <c r="B22" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
@@ -1069,7 +1055,7 @@
         <v>32</v>
       </c>
       <c r="B23" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
@@ -1077,7 +1063,7 @@
         <v>5</v>
       </c>
       <c r="B24" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E24" s="11"/>
     </row>
@@ -1106,8 +1092,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F77FDBE-4564-4278-9755-9E7B4B955105}">
   <dimension ref="A1:G25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>